<commit_message>
Finished sensor programming, added measurements for battery life time estimations
</commit_message>
<xml_diff>
--- a/register_map/input_struct.xlsx
+++ b/register_map/input_struct.xlsx
@@ -88,7 +88,7 @@
     <t xml:space="preserve">a</t>
   </si>
   <si>
-    <t xml:space="preserve">led_en</t>
+    <t xml:space="preserve">led_dis</t>
   </si>
   <si>
     <t xml:space="preserve">Bitwise array: enable LED on each node</t>
@@ -217,10 +217,10 @@
   <dimension ref="A1:U16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="118" zoomScaleNormal="118" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.62"/>

</xml_diff>